<commit_message>
Add ability to extract report type/notes from quarterly reports
</commit_message>
<xml_diff>
--- a/quarterlyReports/mammograms_edited/10-01-20 PCHS Mammogram screening Rate Report.xlsx
+++ b/quarterlyReports/mammograms_edited/10-01-20 PCHS Mammogram screening Rate Report.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mayalapp/Documents/coding_projects/dad_data_project/quarterlyReports/mammograms_edited/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111D5DA6-1403-C042-8C91-18E811840239}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B55AD187-4BF5-924D-8BA2-E56162D873DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="23260" windowHeight="12580" tabRatio="232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -111,16 +111,16 @@
     <t>Report type</t>
   </si>
   <si>
-    <t>Name of report (e.g. "Mammogram screening")</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>All patient notes here</t>
-  </si>
-  <si>
-    <t>Screened patient notes here</t>
+    <t>Mammogram Screening</t>
+  </si>
+  <si>
+    <t>All Patients:  Active Female patients between the 50 and 74 years of age that DID NOT have a mastectomy and that  had a medical visit during the 3 years prior to the end of the reporting period.</t>
+  </si>
+  <si>
+    <t>Screened patients: Patients that received a mammogram during the 2 years prior to the end of the reporting period.</t>
   </si>
 </sst>
 </file>
@@ -925,7 +925,7 @@
   <dimension ref="A1:AB54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.75" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -957,7 +957,7 @@
         <v>25</v>
       </c>
       <c r="B1" s="41" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C1" s="42"/>
       <c r="D1" s="42"/>
@@ -965,7 +965,7 @@
     </row>
     <row r="2" spans="1:28" s="43" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="41" t="s">
         <v>28</v>

</xml_diff>